<commit_message>
Added the countdown track
</commit_message>
<xml_diff>
--- a/Assets/Index.xlsx
+++ b/Assets/Index.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -396,7 +396,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>- Roberto Roena - Tu Loco Loco, Y Yo Tranquilo</t>
+          <t>- Roberto Roena - Tu Loco Loco, Y Yo Tranquilo.mp3</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -407,7 +407,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>01 Asi Es La Mujer</t>
+          <t>01 Asi Es La Mujer.mp3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -418,7 +418,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>01 Buenas Noches Che Che</t>
+          <t>01 Buenas Noches Che Che.mp3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -429,7 +429,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>04 Sun Sun Babae</t>
+          <t>04 Sun Sun Babae.mp3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -440,7 +440,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>09 ramo de rosas</t>
+          <t>09 ramo de rosas.mp3</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -451,7 +451,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3 La Maxima 79 - Kun Kin</t>
+          <t>3 La Maxima 79 - Kun Kin.mp3</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -462,7 +462,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6 La Maxima 79 - Cuchi Cuchi</t>
+          <t>6 La Maxima 79 - Cuchi Cuchi.mp3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -473,7 +473,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Adolescentes - Aquel lugar</t>
+          <t>Adolescentes - Aquel lugar.mp3</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -484,7 +484,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Alfredito Linares - Ain't No Sunshine (1)</t>
+          <t>Alfredito Linares - Ain't No Sunshine (1).mp3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -495,7 +495,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Angel Canales-Hace Tiempo</t>
+          <t>Angel Canales-Hace Tiempo.mp3</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -506,7 +506,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Aventura - Obsesion</t>
+          <t>Aventura - Obsesion.mp3</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -517,7 +517,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aya Nakamura - Djadja </t>
+          <t>Aya Nakamura - Djadja .mp3</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -528,7 +528,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Benny More &amp; Oscar De Leon - Castellano que bueno baila usted</t>
+          <t>Benny More &amp; Oscar De Leon - Castellano que bueno baila usted.mp3</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -539,7 +539,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CAMPANA MAYORAL-JOSE MANGUAL JR</t>
+          <t>CAMPANA MAYORAL-JOSE MANGUAL JR.mp3</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -550,7 +550,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Charlie Palmieri-Tiene Sabor</t>
+          <t>Charlie Palmieri-Tiene Sabor.mp3</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -561,7 +561,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Christian Castro - Azul (merengue)</t>
+          <t>Christian Castro - Azul (merengue).mp3</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -572,7 +572,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Eddie Palmieri - Bailare Tu Son</t>
+          <t>Eddie Palmieri - Bailare Tu Son.mp3</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -583,7 +583,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>El Chaval - Amor Amor</t>
+          <t>El Chaval - Amor Amor.mp3</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -594,7 +594,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Fania All Stars - Ublabadu</t>
+          <t>Fania All Stars - Ublabadu.mp3</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -605,7 +605,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Frank Reyes - Princesa</t>
+          <t>Frank Reyes - Princesa.mp3</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -616,7 +616,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Frank Reyes - Quien eres tu</t>
+          <t>Frank Reyes - Quien eres tu.mp3</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -627,7 +627,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Frank Reyes - Tú eres ajena</t>
+          <t>Frank Reyes - Tú eres ajena.mp3</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -638,7 +638,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Fruko y Sus Yesos - El Preso Original</t>
+          <t>Fruko y Sus Yesos - El Preso Original.mp3</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -649,7 +649,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Gerardo Rosales-Anacaona (directo)</t>
+          <t>Gerardo Rosales-Anacaona (directo).mp3</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -660,7 +660,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Gran combo - El matrimonio</t>
+          <t>Gran combo - El matrimonio.mp3</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -671,7 +671,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Ismael Rivera - Bilongo</t>
+          <t>Index.xlsx</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -682,7 +682,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Joe Cuba - Bang bang</t>
+          <t>Ismael Rivera - Bilongo.mp3</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -693,7 +693,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Johnny Pacheco - Azuquita mami</t>
+          <t>Joe Cuba - Bang bang.mp3</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -704,7 +704,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Juan Luis Guerra - Ay Mujer</t>
+          <t>Johnny Pacheco - Azuquita mami.mp3</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -715,7 +715,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Juan Luis Guerra浯洀 - Señales De Humo</t>
+          <t>Juan Luis Guerra - Ay Mujer.mp3</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -726,7 +726,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>kiko Rodrigues - Hoy Te Vi Pasar</t>
+          <t>Juan Luis Guerra浯洀 - Señales De Humo.mp3</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -737,7 +737,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Kiko Rodriguez - Vagabundo, borracho y loco 2cd (A. Khazin) mp3</t>
+          <t>kiko Rodrigues - Hoy Te Vi Pasar.mp3</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -748,7 +748,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>la nova tradicional - vente negra</t>
+          <t>Kiko Rodriguez - Vagabundo, borracho y loco 2cd (A. Khazin) mp3.mp3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -759,7 +759,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Lalo Rodriguez - Ven, Devorame Otra Vez (Lalo Rodriguez)</t>
+          <t>la nova tradicional - vente negra.mp3</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -770,7 +770,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Leoni Torres Ft Kelvis Ochoa &amp; Alexander Abreu - Es Tu Mirada</t>
+          <t>Lalo Rodriguez - Ven, Devorame Otra Vez (Lalo Rodriguez).mp3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -781,7 +781,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Los Titanes - Merecumbe</t>
+          <t>Leoni Torres Ft Kelvis Ochoa &amp; Alexander Abreu - Es Tu Mirada.mp3</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -792,7 +792,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Luis Miguel De La Amargue - Abrazame Amor</t>
+          <t>Los Titanes - Merecumbe.mp3</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -803,7 +803,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>LUIS MIGUEL DEL AMARGUE - Amor de locos</t>
+          <t>Luis Miguel De La Amargue - Abrazame Amor.mp3</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -814,7 +814,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Manolito Simonet y Su Trabuco - La habana me llama</t>
+          <t>LUIS MIGUEL DEL AMARGUE - Amor de locos.mp3</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -825,7 +825,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Marc Anthony - Te Conozco Bien</t>
+          <t>Manolito Simonet y Su Trabuco - La habana me llama.mp3</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -836,7 +836,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Marc Anthony-Aguanile</t>
+          <t>Marc Anthony - Te Conozco Bien.mp3</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -847,7 +847,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mito Feat Mr Kuka - Que Tal</t>
+          <t>Marc Anthony-Aguanile.mp3</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -858,7 +858,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Monchi y Alexandra - Dos Locos</t>
+          <t>Mito Feat Mr Kuka - Que Tal.mp3</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -869,7 +869,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Monchy &amp; Alexandra - Hasta El Fin</t>
+          <t>Monchi y Alexandra - Dos Locos.mp3</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -880,7 +880,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>New Swing Sextet - Sarandonga mp3</t>
+          <t>Monchy &amp; Alexandra - Hasta El Fin.mp3</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -891,7 +891,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ORQUESTA GUAYACAN--OIGA,MIRA.VEA.</t>
+          <t>New Swing Sextet - Sarandonga mp3.mp3</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -902,7 +902,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Polo Montanez-Cuestion de Suerte</t>
+          <t>ORQUESTA GUAYACAN--OIGA,MIRA.VEA..mp3</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -913,7 +913,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Poncho Sanchez - Guaripumpe</t>
+          <t>Polo Montanez-Cuestion de Suerte.mp3</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -924,7 +924,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Raulin Rodriguez - Y Llorare</t>
+          <t>Poncho Sanchez - Guaripumpe.mp3</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -935,7 +935,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Ray Baretto-Vive y Vacila</t>
+          <t>Raulin Rodriguez - Y Llorare.mp3</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -946,7 +946,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Ray Barreto-Guarare</t>
+          <t>Ray Baretto-Vive y Vacila.mp3</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -957,7 +957,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Ray Pérez - Emae Emae</t>
+          <t>Ray Barreto-Guarare.mp3</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -968,7 +968,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Rey Ruiz - LUNA NEGRA</t>
+          <t>Ray Pérez - Emae Emae.mp3</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -979,7 +979,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Ricardo Ray &amp; Bobby Cruz - Aguzate</t>
+          <t>Rey Ruiz - LUNA NEGRA.mp3</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -990,7 +990,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Ricardo Ray &amp; Bobby Cruz - Sonido Bestial</t>
+          <t>Ricardo Ray &amp; Bobby Cruz - Aguzate.mp3</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1001,7 +1001,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>ruben blades - Amor y Control</t>
+          <t>Ricardo Ray &amp; Bobby Cruz - Sonido Bestial.mp3</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1012,7 +1012,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Salsa Kids - Dejame un Beso</t>
+          <t>ruben blades - Amor y Control.mp3</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1023,7 +1023,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Sonero-Johnny Pacheco</t>
+          <t>Salsa Kids - Dejame un Beso.mp3</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1034,7 +1034,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Sonora Carrusseles - Arranca en Fa</t>
+          <t>Sonero-Johnny Pacheco.mp3</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1045,7 +1045,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Sonora Matancera - Mala mujer</t>
+          <t>Sonora Carrusseles - Arranca en Fa.mp3</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1056,7 +1056,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>The Soca Boys - Follow The Leader</t>
+          <t>Sonora Matancera - Mala mujer.mp3</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1067,7 +1067,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>The Whistler's Song</t>
+          <t>The Soca Boys - Follow The Leader.mp3</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1078,7 +1078,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Tito Allen y Larry Harlow - Silencio (Omelenco Guaguanco)</t>
+          <t>The Whistler's Song.mp3</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1089,7 +1089,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Tito Puente - Oye Como Va</t>
+          <t>Tito Allen y Larry Harlow - Silencio (Omelenco Guaguanco).mp3</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1100,7 +1100,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Tito Puente - Ran Kan Kan</t>
+          <t>Tito Puente - Oye Como Va.mp3</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -1111,7 +1111,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Tito Puente-Mambo gozón</t>
+          <t>Tito Puente - Ran Kan Kan.mp3</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -1122,7 +1122,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Tony Vega - Dejame Soñar</t>
+          <t>Tito Puente-Mambo gozón.mp3</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -1133,7 +1133,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Varios Artistas - Varios Artistas - Willie Rosario - Let's Boogaloo</t>
+          <t>Tony Vega - Dejame Soñar.mp3</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -1144,7 +1144,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Victor Manuelle - He Tratado</t>
+          <t>Varios Artistas - Varios Artistas - Willie Rosario - Let's Boogaloo.mp3</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -1155,7 +1155,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Wayne Gorbea - Lo Que Dice Justi</t>
+          <t>Victor Manuelle - He Tratado.mp3</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -1166,7 +1166,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Zacarias Ferreira - Dame Tu Amor</t>
+          <t>Wayne Gorbea - Lo Que Dice Justi.mp3</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -1177,7 +1177,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Zacarias Ferreira - Sentimiento De Amor</t>
+          <t>Zacarias Ferreira - Dame Tu Amor.mp3</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -1185,6 +1185,17 @@
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
     </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Zacarias Ferreira - Sentimiento De Amor.mp3</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>